<commit_message>
updated figs and analyses
</commit_message>
<xml_diff>
--- a/Data/BiovolumeAfterSettlement.xlsx
+++ b/Data/BiovolumeAfterSettlement.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shelly/Documents/GitHub/paper-OysterSeed-TimeXTemp/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DA9D915-2490-6643-9ED5-184199DED14F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C0C4F8-C08F-EE4D-BD5F-EB12AFCD0567}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1460" windowWidth="24640" windowHeight="14000" xr2:uid="{74195A81-433A-764D-9E62-638FF3AF16AF}"/>
+    <workbookView xWindow="6000" yWindow="3320" windowWidth="24640" windowHeight="14000" xr2:uid="{74195A81-433A-764D-9E62-638FF3AF16AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <r>
       <t>Lower Screen Size (</t>
@@ -182,12 +182,36 @@
   <si>
     <t>Biovolume of oyster seed (mL) settled after 6 days of exposure to high temperatures.  Taylor Shellfish Hatchery provided seed per mL conversions for different screen sizes.</t>
   </si>
+  <si>
+    <r>
+      <t>Screen Size Range (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>m)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -214,6 +238,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -235,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -245,12 +275,23 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE438E4"/>
+      <color rgb="FF00C7C8"/>
+      <color rgb="FF00FDFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -260,6 +301,1084 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16503937007874014"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.80440507436570441"/>
+          <c:h val="0.79500729075532228"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>23°C</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00C7C8"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$4:$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>315-450</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>450-710</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>710-1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000-1320</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1320-1800</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$4:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>143080</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8883</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-C2B6-CB4C-810D-9B2E6872E56D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>29°C</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E438E4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$4:$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>315-450</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>450-710</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>710-1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000-1320</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1320-1800</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$4:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>29827</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78694</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>136000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59220</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5248</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-C2B6-CB4C-810D-9B2E6872E56D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1542258928"/>
+        <c:axId val="1541695520"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1542258928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Screen size (μm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1541695520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1541695520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of oysters</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1542258928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.76603368328958865"/>
+          <c:y val="6.5392971711869349E-2"/>
+          <c:w val="0.17771706152134387"/>
+          <c:h val="7.8269405929095412E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>678302</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>174439</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>306027</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>67797</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FDC8984-18D2-E145-8D2F-93AADCDFCC2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,13 +1678,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22DCC67F-A92E-A846-BAC3-FEE4EDEB1F22}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
@@ -574,12 +1693,12 @@
     <col min="6" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="40" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="37">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -587,137 +1706,161 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>315</v>
       </c>
       <c r="B4" s="1">
         <v>450</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="5" t="str">
+        <f>CONCATENATE(A4,"-",B4)</f>
+        <v>315-450</v>
+      </c>
+      <c r="D4" s="1">
         <v>5423</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>6.5</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>5.5</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="6">
         <v>35250</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="6">
         <v>29827</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>450</v>
       </c>
       <c r="B5" s="1">
         <v>710</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="5" t="str">
+        <f t="shared" ref="C5:C8" si="0">CONCATENATE(A5,"-",B5)</f>
+        <v>450-710</v>
+      </c>
+      <c r="D5" s="1">
         <v>3577</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>40</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>22</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="6">
         <v>143080</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="6">
         <v>78694</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>710</v>
       </c>
       <c r="B6" s="1">
         <v>1000</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>710-1000</v>
+      </c>
+      <c r="D6" s="1">
         <v>2000</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>55</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>68</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="6">
         <v>110000</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="6">
         <v>136000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>1000</v>
       </c>
       <c r="B7" s="1">
         <v>1320</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>1000-1320</v>
+      </c>
+      <c r="D7" s="1">
         <v>846</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>10.5</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>70</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="6">
         <v>8883</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="6">
         <v>59220</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>1320</v>
       </c>
       <c r="B8" s="1">
         <v>1800</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>1320-1800</v>
+      </c>
+      <c r="D8" s="1">
         <v>290</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>18</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="6">
         <v>5248</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>